<commit_message>
Refactor auth code system - remove group column, fix upload UI, remove auth codes from team table, disable auto-generation
</commit_message>
<xml_diff>
--- a/auth-codes.xlsx
+++ b/auth-codes.xlsx
@@ -397,17 +397,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F103"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" customWidth="1" width="8"/>
     <col min="2" max="2" customWidth="1" width="25"/>
-    <col min="3" max="3" customWidth="1" width="5"/>
-    <col min="4" max="4" customWidth="1" width="10"/>
-    <col min="5" max="5" customWidth="1" width="20"/>
-    <col min="6" max="6" customWidth="1" width="12"/>
+    <col min="3" max="3" customWidth="1" width="10"/>
+    <col min="4" max="4" customWidth="1" width="20"/>
+    <col min="5" max="5" customWidth="1" width="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -418,15 +417,12 @@
         <v>팀명</v>
       </c>
       <c r="C1" t="str">
-        <v>그룹</v>
+        <v>멤버 구분</v>
       </c>
       <c r="D1" t="str">
-        <v>멤버 구분</v>
+        <v>LDAP 닉네임</v>
       </c>
       <c r="E1" t="str">
-        <v>LDAP 닉네임</v>
-      </c>
-      <c r="F1" t="str">
         <v>인증 번호</v>
       </c>
     </row>
@@ -438,16 +434,13 @@
         <v>법대로 합시다</v>
       </c>
       <c r="C2" t="str">
-        <v>A</v>
+        <v>팀장</v>
       </c>
       <c r="D2" t="str">
-        <v>팀장</v>
+        <v>logan.g</v>
       </c>
       <c r="E2" t="str">
-        <v>logan.g</v>
-      </c>
-      <c r="F2" t="str">
-        <v>133273</v>
+        <v/>
       </c>
     </row>
     <row r="3">
@@ -458,16 +451,13 @@
         <v>법대로 합시다</v>
       </c>
       <c r="C3" t="str">
-        <v>A</v>
+        <v>팀원2</v>
       </c>
       <c r="D3" t="str">
-        <v>팀원2</v>
+        <v>oregon.a</v>
       </c>
       <c r="E3" t="str">
-        <v>oregon.a</v>
-      </c>
-      <c r="F3" t="str">
-        <v>563344</v>
+        <v/>
       </c>
     </row>
     <row r="4">
@@ -478,16 +468,13 @@
         <v>법대로 합시다</v>
       </c>
       <c r="C4" t="str">
-        <v>A</v>
+        <v>팀원3</v>
       </c>
       <c r="D4" t="str">
-        <v>팀원3</v>
+        <v>alicia.a</v>
       </c>
       <c r="E4" t="str">
-        <v>alicia.a</v>
-      </c>
-      <c r="F4" t="str">
-        <v>346303</v>
+        <v/>
       </c>
     </row>
     <row r="5">
@@ -498,16 +485,13 @@
         <v>법대로 합시다</v>
       </c>
       <c r="C5" t="str">
-        <v>A</v>
+        <v>팀원4</v>
       </c>
       <c r="D5" t="str">
-        <v>팀원4</v>
+        <v>sean.baek</v>
       </c>
       <c r="E5" t="str">
-        <v>sean.baek</v>
-      </c>
-      <c r="F5" t="str">
-        <v>194168</v>
+        <v/>
       </c>
     </row>
     <row r="6">
@@ -518,16 +502,13 @@
         <v>피즈</v>
       </c>
       <c r="C6" t="str">
-        <v>A</v>
+        <v>팀장</v>
       </c>
       <c r="D6" t="str">
-        <v>팀장</v>
+        <v>leo.bing</v>
       </c>
       <c r="E6" t="str">
-        <v>leo.bing</v>
-      </c>
-      <c r="F6" t="str">
-        <v>938302</v>
+        <v/>
       </c>
     </row>
     <row r="7">
@@ -538,16 +519,13 @@
         <v>봄바람</v>
       </c>
       <c r="C7" t="str">
-        <v>A</v>
+        <v>팀장</v>
       </c>
       <c r="D7" t="str">
-        <v>팀장</v>
+        <v>ryder.wind</v>
       </c>
       <c r="E7" t="str">
-        <v>ryder.wind</v>
-      </c>
-      <c r="F7" t="str">
-        <v>821048</v>
+        <v/>
       </c>
     </row>
     <row r="8">
@@ -558,16 +536,13 @@
         <v>봄바람</v>
       </c>
       <c r="C8" t="str">
-        <v>A</v>
+        <v>팀원2</v>
       </c>
       <c r="D8" t="str">
-        <v>팀원2</v>
+        <v>tak.haru</v>
       </c>
       <c r="E8" t="str">
-        <v>tak.haru</v>
-      </c>
-      <c r="F8" t="str">
-        <v>505739</v>
+        <v/>
       </c>
     </row>
     <row r="9">
@@ -578,16 +553,13 @@
         <v>봄바람</v>
       </c>
       <c r="C9" t="str">
-        <v>A</v>
+        <v>팀원3</v>
       </c>
       <c r="D9" t="str">
-        <v>팀원3</v>
+        <v>lou.j</v>
       </c>
       <c r="E9" t="str">
-        <v>lou.j</v>
-      </c>
-      <c r="F9" t="str">
-        <v>794760</v>
+        <v/>
       </c>
     </row>
     <row r="10">
@@ -598,16 +570,13 @@
         <v>봄바람</v>
       </c>
       <c r="C10" t="str">
-        <v>A</v>
+        <v>팀원4</v>
       </c>
       <c r="D10" t="str">
-        <v>팀원4</v>
+        <v>james.yu</v>
       </c>
       <c r="E10" t="str">
-        <v>james.yu</v>
-      </c>
-      <c r="F10" t="str">
-        <v>784908</v>
+        <v/>
       </c>
     </row>
     <row r="11">
@@ -618,16 +587,13 @@
         <v>오메유</v>
       </c>
       <c r="C11" t="str">
-        <v>A</v>
+        <v>팀장</v>
       </c>
       <c r="D11" t="str">
-        <v>팀장</v>
+        <v>miles.stone</v>
       </c>
       <c r="E11" t="str">
-        <v>miles.stone</v>
-      </c>
-      <c r="F11" t="str">
-        <v>457589</v>
+        <v/>
       </c>
     </row>
     <row r="12">
@@ -638,16 +604,13 @@
         <v>오메유</v>
       </c>
       <c r="C12" t="str">
-        <v>A</v>
+        <v>팀원2</v>
       </c>
       <c r="D12" t="str">
-        <v>팀원2</v>
+        <v>ogong.cloud</v>
       </c>
       <c r="E12" t="str">
-        <v>ogong.cloud</v>
-      </c>
-      <c r="F12" t="str">
-        <v>769622</v>
+        <v/>
       </c>
     </row>
     <row r="13">
@@ -658,16 +621,13 @@
         <v>오메유</v>
       </c>
       <c r="C13" t="str">
-        <v>A</v>
+        <v>팀원3</v>
       </c>
       <c r="D13" t="str">
-        <v>팀원3</v>
+        <v>eli.94</v>
       </c>
       <c r="E13" t="str">
-        <v>eli.94</v>
-      </c>
-      <c r="F13" t="str">
-        <v>200003</v>
+        <v/>
       </c>
     </row>
     <row r="14">
@@ -678,16 +638,13 @@
         <v>오메유</v>
       </c>
       <c r="C14" t="str">
-        <v>A</v>
+        <v>팀원4</v>
       </c>
       <c r="D14" t="str">
-        <v>팀원4</v>
+        <v>ud.zip</v>
       </c>
       <c r="E14" t="str">
-        <v>ud.zip</v>
-      </c>
-      <c r="F14" t="str">
-        <v>828570</v>
+        <v/>
       </c>
     </row>
     <row r="15">
@@ -698,16 +655,13 @@
         <v>닝닝.ai</v>
       </c>
       <c r="C15" t="str">
-        <v>A</v>
+        <v>팀장</v>
       </c>
       <c r="D15" t="str">
-        <v>팀장</v>
+        <v>lucas.nova</v>
       </c>
       <c r="E15" t="str">
-        <v>lucas.nova</v>
-      </c>
-      <c r="F15" t="str">
-        <v>912915</v>
+        <v/>
       </c>
     </row>
     <row r="16">
@@ -718,16 +672,13 @@
         <v>닝닝.ai</v>
       </c>
       <c r="C16" t="str">
-        <v>A</v>
+        <v>팀원2</v>
       </c>
       <c r="D16" t="str">
-        <v>팀원2</v>
+        <v>joy.wooyakko</v>
       </c>
       <c r="E16" t="str">
-        <v>joy.wooyakko</v>
-      </c>
-      <c r="F16" t="str">
-        <v>662817</v>
+        <v/>
       </c>
     </row>
     <row r="17">
@@ -738,16 +689,13 @@
         <v>닝닝.ai</v>
       </c>
       <c r="C17" t="str">
-        <v>A</v>
+        <v>팀원3</v>
       </c>
       <c r="D17" t="str">
-        <v>팀원3</v>
+        <v>jackson.yoon</v>
       </c>
       <c r="E17" t="str">
-        <v>jackson.yoon</v>
-      </c>
-      <c r="F17" t="str">
-        <v>148249</v>
+        <v/>
       </c>
     </row>
     <row r="18">
@@ -758,16 +706,13 @@
         <v>KVP</v>
       </c>
       <c r="C18" t="str">
-        <v>A</v>
+        <v>팀장</v>
       </c>
       <c r="D18" t="str">
-        <v>팀장</v>
+        <v>evin.yj</v>
       </c>
       <c r="E18" t="str">
-        <v>evin.yj</v>
-      </c>
-      <c r="F18" t="str">
-        <v>913457</v>
+        <v/>
       </c>
     </row>
     <row r="19">
@@ -778,16 +723,13 @@
         <v>KVP</v>
       </c>
       <c r="C19" t="str">
-        <v>A</v>
+        <v>팀원2</v>
       </c>
       <c r="D19" t="str">
-        <v>팀원2</v>
+        <v>vito.kim</v>
       </c>
       <c r="E19" t="str">
-        <v>vito.kim</v>
-      </c>
-      <c r="F19" t="str">
-        <v>988170</v>
+        <v/>
       </c>
     </row>
     <row r="20">
@@ -798,16 +740,13 @@
         <v>데엔이지만 AI는 하고 싶어!</v>
       </c>
       <c r="C20" t="str">
-        <v>A</v>
+        <v>팀장</v>
       </c>
       <c r="D20" t="str">
-        <v>팀장</v>
+        <v>nyx.domi</v>
       </c>
       <c r="E20" t="str">
-        <v>nyx.domi</v>
-      </c>
-      <c r="F20" t="str">
-        <v>745942</v>
+        <v/>
       </c>
     </row>
     <row r="21">
@@ -818,16 +757,13 @@
         <v>데엔이지만 AI는 하고 싶어!</v>
       </c>
       <c r="C21" t="str">
-        <v>A</v>
+        <v>팀원2</v>
       </c>
       <c r="D21" t="str">
-        <v>팀원2</v>
+        <v>ian.hyuek</v>
       </c>
       <c r="E21" t="str">
-        <v>ian.hyuek</v>
-      </c>
-      <c r="F21" t="str">
-        <v>550316</v>
+        <v/>
       </c>
     </row>
     <row r="22">
@@ -838,16 +774,13 @@
         <v>데엔이지만 AI는 하고 싶어!</v>
       </c>
       <c r="C22" t="str">
-        <v>A</v>
+        <v>팀원3</v>
       </c>
       <c r="D22" t="str">
-        <v>팀원3</v>
+        <v>gide.yso</v>
       </c>
       <c r="E22" t="str">
-        <v>gide.yso</v>
-      </c>
-      <c r="F22" t="str">
-        <v>440444</v>
+        <v/>
       </c>
     </row>
     <row r="23">
@@ -858,16 +791,13 @@
         <v>데엔이지만 AI는 하고 싶어!</v>
       </c>
       <c r="C23" t="str">
-        <v>A</v>
+        <v>팀원4</v>
       </c>
       <c r="D23" t="str">
-        <v>팀원4</v>
+        <v>rian.bow</v>
       </c>
       <c r="E23" t="str">
-        <v>rian.bow</v>
-      </c>
-      <c r="F23" t="str">
-        <v>928950</v>
+        <v/>
       </c>
     </row>
     <row r="24">
@@ -878,16 +808,13 @@
         <v>나는솔로</v>
       </c>
       <c r="C24" t="str">
-        <v>A</v>
+        <v>팀장</v>
       </c>
       <c r="D24" t="str">
-        <v>팀장</v>
+        <v>bacchus.f</v>
       </c>
       <c r="E24" t="str">
-        <v>bacchus.f</v>
-      </c>
-      <c r="F24" t="str">
-        <v>358162</v>
+        <v/>
       </c>
     </row>
     <row r="25">
@@ -898,16 +825,13 @@
         <v>스테릭의단검</v>
       </c>
       <c r="C25" t="str">
-        <v>A</v>
+        <v>팀장</v>
       </c>
       <c r="D25" t="str">
-        <v>팀장</v>
+        <v>derek.young</v>
       </c>
       <c r="E25" t="str">
-        <v>derek.young</v>
-      </c>
-      <c r="F25" t="str">
-        <v>114196</v>
+        <v/>
       </c>
     </row>
     <row r="26">
@@ -918,16 +842,13 @@
         <v>스테릭의단검</v>
       </c>
       <c r="C26" t="str">
-        <v>A</v>
+        <v>팀원2</v>
       </c>
       <c r="D26" t="str">
-        <v>팀원2</v>
+        <v>steve.play</v>
       </c>
       <c r="E26" t="str">
-        <v>steve.play</v>
-      </c>
-      <c r="F26" t="str">
-        <v>589234</v>
+        <v/>
       </c>
     </row>
     <row r="27">
@@ -938,16 +859,13 @@
         <v>스테릭의단검</v>
       </c>
       <c r="C27" t="str">
-        <v>A</v>
+        <v>팀원3</v>
       </c>
       <c r="D27" t="str">
-        <v>팀원3</v>
+        <v>terra.bite</v>
       </c>
       <c r="E27" t="str">
-        <v>terra.bite</v>
-      </c>
-      <c r="F27" t="str">
-        <v>596673</v>
+        <v/>
       </c>
     </row>
     <row r="28">
@@ -958,16 +876,13 @@
         <v>스테릭의단검</v>
       </c>
       <c r="C28" t="str">
-        <v>A</v>
+        <v>팀원4</v>
       </c>
       <c r="D28" t="str">
-        <v>팀원4</v>
+        <v>khloe.wynn</v>
       </c>
       <c r="E28" t="str">
-        <v>khloe.wynn</v>
-      </c>
-      <c r="F28" t="str">
-        <v>254899</v>
+        <v/>
       </c>
     </row>
     <row r="29">
@@ -978,16 +893,13 @@
         <v>배휴~나?</v>
       </c>
       <c r="C29" t="str">
-        <v>A</v>
+        <v>팀장</v>
       </c>
       <c r="D29" t="str">
-        <v>팀장</v>
+        <v>hugh.1123</v>
       </c>
       <c r="E29" t="str">
-        <v>hugh.1123</v>
-      </c>
-      <c r="F29" t="str">
-        <v>538628</v>
+        <v/>
       </c>
     </row>
     <row r="30">
@@ -998,16 +910,13 @@
         <v>배휴~나?</v>
       </c>
       <c r="C30" t="str">
-        <v>A</v>
+        <v>팀원2</v>
       </c>
       <c r="D30" t="str">
-        <v>팀원2</v>
+        <v>lina.a</v>
       </c>
       <c r="E30" t="str">
-        <v>lina.a</v>
-      </c>
-      <c r="F30" t="str">
-        <v>381887</v>
+        <v/>
       </c>
     </row>
     <row r="31">
@@ -1018,16 +927,13 @@
         <v>배휴~나?</v>
       </c>
       <c r="C31" t="str">
-        <v>A</v>
+        <v>팀원3</v>
       </c>
       <c r="D31" t="str">
-        <v>팀원3</v>
+        <v>bell.na</v>
       </c>
       <c r="E31" t="str">
-        <v>bell.na</v>
-      </c>
-      <c r="F31" t="str">
-        <v>907698</v>
+        <v/>
       </c>
     </row>
     <row r="32">
@@ -1038,16 +944,13 @@
         <v>아말감</v>
       </c>
       <c r="C32" t="str">
-        <v>B</v>
+        <v>팀장</v>
       </c>
       <c r="D32" t="str">
-        <v>팀장</v>
+        <v>woody.n</v>
       </c>
       <c r="E32" t="str">
-        <v>woody.n</v>
-      </c>
-      <c r="F32" t="str">
-        <v>955688</v>
+        <v/>
       </c>
     </row>
     <row r="33">
@@ -1058,16 +961,13 @@
         <v>아말감</v>
       </c>
       <c r="C33" t="str">
-        <v>B</v>
+        <v>팀원2</v>
       </c>
       <c r="D33" t="str">
-        <v>팀원2</v>
+        <v>rick.9</v>
       </c>
       <c r="E33" t="str">
-        <v>rick.9</v>
-      </c>
-      <c r="F33" t="str">
-        <v>578198</v>
+        <v/>
       </c>
     </row>
     <row r="34">
@@ -1078,16 +978,13 @@
         <v>아말감</v>
       </c>
       <c r="C34" t="str">
-        <v>B</v>
+        <v>팀원3</v>
       </c>
       <c r="D34" t="str">
-        <v>팀원3</v>
+        <v>peter.hoon</v>
       </c>
       <c r="E34" t="str">
-        <v>peter.hoon</v>
-      </c>
-      <c r="F34" t="str">
-        <v>399937</v>
+        <v/>
       </c>
     </row>
     <row r="35">
@@ -1098,16 +995,13 @@
         <v>아말감</v>
       </c>
       <c r="C35" t="str">
-        <v>B</v>
+        <v>팀원4</v>
       </c>
       <c r="D35" t="str">
-        <v>팀원4</v>
+        <v>adam.min</v>
       </c>
       <c r="E35" t="str">
-        <v>adam.min</v>
-      </c>
-      <c r="F35" t="str">
-        <v>144006</v>
+        <v/>
       </c>
     </row>
     <row r="36">
@@ -1118,16 +1012,13 @@
         <v>모아모아</v>
       </c>
       <c r="C36" t="str">
-        <v>B</v>
+        <v>팀장</v>
       </c>
       <c r="D36" t="str">
-        <v>팀장</v>
+        <v>maison.sun</v>
       </c>
       <c r="E36" t="str">
-        <v>maison.sun</v>
-      </c>
-      <c r="F36" t="str">
-        <v>825295</v>
+        <v/>
       </c>
     </row>
     <row r="37">
@@ -1138,16 +1029,13 @@
         <v>모아모아</v>
       </c>
       <c r="C37" t="str">
-        <v>B</v>
+        <v>팀원2</v>
       </c>
       <c r="D37" t="str">
-        <v>팀원2</v>
+        <v>aaron.bless</v>
       </c>
       <c r="E37" t="str">
-        <v>aaron.bless</v>
-      </c>
-      <c r="F37" t="str">
-        <v>522149</v>
+        <v/>
       </c>
     </row>
     <row r="38">
@@ -1158,16 +1046,13 @@
         <v>모아모아</v>
       </c>
       <c r="C38" t="str">
-        <v>B</v>
+        <v>팀원3</v>
       </c>
       <c r="D38" t="str">
-        <v>팀원3</v>
+        <v>andrew.j88</v>
       </c>
       <c r="E38" t="str">
-        <v>andrew.j88</v>
-      </c>
-      <c r="F38" t="str">
-        <v>954411</v>
+        <v/>
       </c>
     </row>
     <row r="39">
@@ -1178,16 +1063,13 @@
         <v>모아모아</v>
       </c>
       <c r="C39" t="str">
-        <v>B</v>
+        <v>팀원4</v>
       </c>
       <c r="D39" t="str">
-        <v>팀원4</v>
+        <v>harry.2024</v>
       </c>
       <c r="E39" t="str">
-        <v>harry.2024</v>
-      </c>
-      <c r="F39" t="str">
-        <v>121596</v>
+        <v/>
       </c>
     </row>
     <row r="40">
@@ -1198,16 +1080,13 @@
         <v>슬기로운AI생활</v>
       </c>
       <c r="C40" t="str">
-        <v>B</v>
+        <v>팀장</v>
       </c>
       <c r="D40" t="str">
-        <v>팀장</v>
+        <v>john.al</v>
       </c>
       <c r="E40" t="str">
-        <v>john.ai</v>
-      </c>
-      <c r="F40" t="str">
-        <v>882776</v>
+        <v/>
       </c>
     </row>
     <row r="41">
@@ -1218,16 +1097,13 @@
         <v>슬기로운AI생활</v>
       </c>
       <c r="C41" t="str">
-        <v>B</v>
+        <v>팀원2</v>
       </c>
       <c r="D41" t="str">
-        <v>팀원2</v>
+        <v>bella.nam</v>
       </c>
       <c r="E41" t="str">
-        <v>bella.nam</v>
-      </c>
-      <c r="F41" t="str">
-        <v>289878</v>
+        <v/>
       </c>
     </row>
     <row r="42">
@@ -1238,16 +1114,13 @@
         <v>슬기로운AI생활</v>
       </c>
       <c r="C42" t="str">
-        <v>B</v>
+        <v>팀원3</v>
       </c>
       <c r="D42" t="str">
-        <v>팀원3</v>
+        <v>ico.dev</v>
       </c>
       <c r="E42" t="str">
-        <v>ico.dev</v>
-      </c>
-      <c r="F42" t="str">
-        <v>753684</v>
+        <v/>
       </c>
     </row>
     <row r="43">
@@ -1258,16 +1131,13 @@
         <v>슬기로운AI생활</v>
       </c>
       <c r="C43" t="str">
-        <v>B</v>
+        <v>팀원4</v>
       </c>
       <c r="D43" t="str">
-        <v>팀원4</v>
+        <v>danny.l</v>
       </c>
       <c r="E43" t="str">
-        <v>danny.l</v>
-      </c>
-      <c r="F43" t="str">
-        <v>726566</v>
+        <v/>
       </c>
     </row>
     <row r="44">
@@ -1278,16 +1148,13 @@
         <v>잡았다요놈</v>
       </c>
       <c r="C44" t="str">
-        <v>B</v>
+        <v>팀장</v>
       </c>
       <c r="D44" t="str">
-        <v>팀장</v>
+        <v>jaclyn.n</v>
       </c>
       <c r="E44" t="str">
-        <v>jaclyn.n</v>
-      </c>
-      <c r="F44" t="str">
-        <v>490873</v>
+        <v/>
       </c>
     </row>
     <row r="45">
@@ -1298,16 +1165,13 @@
         <v>잡았다요놈</v>
       </c>
       <c r="C45" t="str">
-        <v>B</v>
+        <v>팀원2</v>
       </c>
       <c r="D45" t="str">
-        <v>팀원2</v>
+        <v>lucas.link</v>
       </c>
       <c r="E45" t="str">
-        <v>lucas.link</v>
-      </c>
-      <c r="F45" t="str">
-        <v>928813</v>
+        <v/>
       </c>
     </row>
     <row r="46">
@@ -1318,16 +1182,13 @@
         <v>잡았다요놈</v>
       </c>
       <c r="C46" t="str">
-        <v>B</v>
+        <v>팀원3</v>
       </c>
       <c r="D46" t="str">
-        <v>팀원3</v>
+        <v>cyan.jade</v>
       </c>
       <c r="E46" t="str">
-        <v>cyan.jade</v>
-      </c>
-      <c r="F46" t="str">
-        <v>571299</v>
+        <v/>
       </c>
     </row>
     <row r="47">
@@ -1338,16 +1199,13 @@
         <v>잡았다요놈</v>
       </c>
       <c r="C47" t="str">
-        <v>B</v>
+        <v>팀원4</v>
       </c>
       <c r="D47" t="str">
-        <v>팀원4</v>
+        <v>theo.jo</v>
       </c>
       <c r="E47" t="str">
-        <v>theo.jo</v>
-      </c>
-      <c r="F47" t="str">
-        <v>551588</v>
+        <v/>
       </c>
     </row>
     <row r="48">
@@ -1358,16 +1216,13 @@
         <v>두뇌작당</v>
       </c>
       <c r="C48" t="str">
-        <v>B</v>
+        <v>팀장</v>
       </c>
       <c r="D48" t="str">
-        <v>팀장</v>
+        <v>jor.dy</v>
       </c>
       <c r="E48" t="str">
-        <v>jor.dy</v>
-      </c>
-      <c r="F48" t="str">
-        <v>808683</v>
+        <v/>
       </c>
     </row>
     <row r="49">
@@ -1378,16 +1233,13 @@
         <v>두뇌작당</v>
       </c>
       <c r="C49" t="str">
-        <v>B</v>
+        <v>팀원2</v>
       </c>
       <c r="D49" t="str">
-        <v>팀원2</v>
+        <v>walker.kind</v>
       </c>
       <c r="E49" t="str">
-        <v>walker.kind</v>
-      </c>
-      <c r="F49" t="str">
-        <v>373900</v>
+        <v/>
       </c>
     </row>
     <row r="50">
@@ -1398,16 +1250,13 @@
         <v>두뇌작당</v>
       </c>
       <c r="C50" t="str">
-        <v>B</v>
+        <v>팀원3</v>
       </c>
       <c r="D50" t="str">
-        <v>팀원3</v>
+        <v>orsay.art</v>
       </c>
       <c r="E50" t="str">
-        <v>orsay.art</v>
-      </c>
-      <c r="F50" t="str">
-        <v>453216</v>
+        <v/>
       </c>
     </row>
     <row r="51">
@@ -1418,16 +1267,13 @@
         <v>존네좋은공시생활</v>
       </c>
       <c r="C51" t="str">
-        <v>B</v>
+        <v>팀장</v>
       </c>
       <c r="D51" t="str">
-        <v>팀장</v>
+        <v>john.athan</v>
       </c>
       <c r="E51" t="str">
-        <v>john.athan</v>
-      </c>
-      <c r="F51" t="str">
-        <v>247495</v>
+        <v/>
       </c>
     </row>
     <row r="52">
@@ -1438,16 +1284,13 @@
         <v>존네좋은공시생활</v>
       </c>
       <c r="C52" t="str">
-        <v>B</v>
+        <v>팀원2</v>
       </c>
       <c r="D52" t="str">
-        <v>팀원2</v>
+        <v>erin.u</v>
       </c>
       <c r="E52" t="str">
-        <v>erin.u</v>
-      </c>
-      <c r="F52" t="str">
-        <v>596076</v>
+        <v/>
       </c>
     </row>
     <row r="53">
@@ -1458,16 +1301,13 @@
         <v>존네좋은공시생활</v>
       </c>
       <c r="C53" t="str">
-        <v>B</v>
+        <v>팀원3</v>
       </c>
       <c r="D53" t="str">
-        <v>팀원3</v>
+        <v>sean.cm</v>
       </c>
       <c r="E53" t="str">
-        <v>sean.cm</v>
-      </c>
-      <c r="F53" t="str">
-        <v>759463</v>
+        <v/>
       </c>
     </row>
     <row r="54">
@@ -1478,16 +1318,13 @@
         <v>존네좋은공시생활</v>
       </c>
       <c r="C54" t="str">
-        <v>B</v>
+        <v>팀원4</v>
       </c>
       <c r="D54" t="str">
-        <v>팀원4</v>
+        <v>zero.a</v>
       </c>
       <c r="E54" t="str">
-        <v>zero.a</v>
-      </c>
-      <c r="F54" t="str">
-        <v>843363</v>
+        <v/>
       </c>
     </row>
     <row r="55">
@@ -1498,16 +1335,13 @@
         <v>캐시미이프유캔(Cash Me if you can)</v>
       </c>
       <c r="C55" t="str">
-        <v>B</v>
+        <v>팀장</v>
       </c>
       <c r="D55" t="str">
-        <v>팀장</v>
+        <v>barack.abama</v>
       </c>
       <c r="E55" t="str">
-        <v>barack.abama</v>
-      </c>
-      <c r="F55" t="str">
-        <v>231832</v>
+        <v/>
       </c>
     </row>
     <row r="56">
@@ -1518,16 +1352,13 @@
         <v>캐시미이프유캔(Cash Me if you can)</v>
       </c>
       <c r="C56" t="str">
-        <v>B</v>
+        <v>팀원2</v>
       </c>
       <c r="D56" t="str">
-        <v>팀원2</v>
+        <v>heidi.0929</v>
       </c>
       <c r="E56" t="str">
-        <v>heidi.0929</v>
-      </c>
-      <c r="F56" t="str">
-        <v>676584</v>
+        <v/>
       </c>
     </row>
     <row r="57">
@@ -1538,16 +1369,13 @@
         <v>캐시미이프유캔(Cash Me if you can)</v>
       </c>
       <c r="C57" t="str">
-        <v>B</v>
+        <v>팀원3</v>
       </c>
       <c r="D57" t="str">
-        <v>팀원3</v>
+        <v>marc.shin</v>
       </c>
       <c r="E57" t="str">
-        <v>marc.shin</v>
-      </c>
-      <c r="F57" t="str">
-        <v>512794</v>
+        <v/>
       </c>
     </row>
     <row r="58">
@@ -1558,16 +1386,13 @@
         <v>캐시미이프유캔(Cash Me if you can)</v>
       </c>
       <c r="C58" t="str">
-        <v>B</v>
+        <v>팀원4</v>
       </c>
       <c r="D58" t="str">
-        <v>팀원4</v>
+        <v>brett.bang</v>
       </c>
       <c r="E58" t="str">
-        <v>brett.bang</v>
-      </c>
-      <c r="F58" t="str">
-        <v>543527</v>
+        <v/>
       </c>
     </row>
     <row r="59">
@@ -1578,16 +1403,13 @@
         <v>안카밀로</v>
       </c>
       <c r="C59" t="str">
-        <v>B</v>
+        <v>팀장</v>
       </c>
       <c r="D59" t="str">
-        <v>팀장</v>
+        <v>anna.iam</v>
       </c>
       <c r="E59" t="str">
-        <v>anna.iam</v>
-      </c>
-      <c r="F59" t="str">
-        <v>568391</v>
+        <v/>
       </c>
     </row>
     <row r="60">
@@ -1598,16 +1420,13 @@
         <v>안카밀로</v>
       </c>
       <c r="C60" t="str">
-        <v>B</v>
+        <v>팀원2</v>
       </c>
       <c r="D60" t="str">
-        <v>팀원2</v>
+        <v>kaya.daystar</v>
       </c>
       <c r="E60" t="str">
-        <v>kaya.daystar</v>
-      </c>
-      <c r="F60" t="str">
-        <v>291707</v>
+        <v/>
       </c>
     </row>
     <row r="61">
@@ -1618,16 +1437,13 @@
         <v>안카밀로</v>
       </c>
       <c r="C61" t="str">
-        <v>B</v>
+        <v>팀원3</v>
       </c>
       <c r="D61" t="str">
-        <v>팀원3</v>
+        <v>rose.viva</v>
       </c>
       <c r="E61" t="str">
-        <v>rose.viva</v>
-      </c>
-      <c r="F61" t="str">
-        <v>184151</v>
+        <v/>
       </c>
     </row>
     <row r="62">
@@ -1638,16 +1454,13 @@
         <v>안카밀로</v>
       </c>
       <c r="C62" t="str">
-        <v>B</v>
+        <v>팀원4</v>
       </c>
       <c r="D62" t="str">
-        <v>팀원4</v>
+        <v>millie.y</v>
       </c>
       <c r="E62" t="str">
-        <v>millie.y</v>
-      </c>
-      <c r="F62" t="str">
-        <v>530276</v>
+        <v/>
       </c>
     </row>
     <row r="63">
@@ -1658,16 +1471,13 @@
         <v>NTX</v>
       </c>
       <c r="C63" t="str">
-        <v>B</v>
+        <v>팀장</v>
       </c>
       <c r="D63" t="str">
-        <v>팀장</v>
+        <v>halang.g</v>
       </c>
       <c r="E63" t="str">
-        <v>halang.g</v>
-      </c>
-      <c r="F63" t="str">
-        <v>408599</v>
+        <v/>
       </c>
     </row>
     <row r="64">
@@ -1678,16 +1488,13 @@
         <v>NTX</v>
       </c>
       <c r="C64" t="str">
-        <v>B</v>
+        <v>팀원2</v>
       </c>
       <c r="D64" t="str">
-        <v>팀원2</v>
+        <v>thru.shine</v>
       </c>
       <c r="E64" t="str">
-        <v>thru.shine</v>
-      </c>
-      <c r="F64" t="str">
-        <v>552231</v>
+        <v/>
       </c>
     </row>
     <row r="65">
@@ -1698,16 +1505,13 @@
         <v>NTX</v>
       </c>
       <c r="C65" t="str">
-        <v>B</v>
+        <v>팀원3</v>
       </c>
       <c r="D65" t="str">
-        <v>팀원3</v>
+        <v>ellen.aries</v>
       </c>
       <c r="E65" t="str">
-        <v>ellen.aries</v>
-      </c>
-      <c r="F65" t="str">
-        <v>738960</v>
+        <v/>
       </c>
     </row>
     <row r="66">
@@ -1718,16 +1522,13 @@
         <v>피넛버터</v>
       </c>
       <c r="C66" t="str">
-        <v>B</v>
+        <v>팀장</v>
       </c>
       <c r="D66" t="str">
-        <v>팀장</v>
+        <v>jerome.u</v>
       </c>
       <c r="E66" t="str">
-        <v>jerome.u</v>
-      </c>
-      <c r="F66" t="str">
-        <v>840370</v>
+        <v/>
       </c>
     </row>
     <row r="67">
@@ -1738,16 +1539,13 @@
         <v>피넛버터</v>
       </c>
       <c r="C67" t="str">
-        <v>B</v>
+        <v>팀원2</v>
       </c>
       <c r="D67" t="str">
-        <v>팀원2</v>
+        <v>leo.v</v>
       </c>
       <c r="E67" t="str">
-        <v>leo.v</v>
-      </c>
-      <c r="F67" t="str">
-        <v>719862</v>
+        <v/>
       </c>
     </row>
     <row r="68">
@@ -1758,16 +1556,13 @@
         <v>피넛버터</v>
       </c>
       <c r="C68" t="str">
-        <v>B</v>
+        <v>팀원3</v>
       </c>
       <c r="D68" t="str">
-        <v>팀원3</v>
+        <v>jayden.hue</v>
       </c>
       <c r="E68" t="str">
-        <v>jayden.hue</v>
-      </c>
-      <c r="F68" t="str">
-        <v>422945</v>
+        <v/>
       </c>
     </row>
     <row r="69">
@@ -1778,16 +1573,13 @@
         <v>포킹(four king)</v>
       </c>
       <c r="C69" t="str">
-        <v>B</v>
+        <v>팀장</v>
       </c>
       <c r="D69" t="str">
-        <v>팀장</v>
+        <v>sienna.on</v>
       </c>
       <c r="E69" t="str">
-        <v>sienna.on</v>
-      </c>
-      <c r="F69" t="str">
-        <v>736727</v>
+        <v/>
       </c>
     </row>
     <row r="70">
@@ -1798,16 +1590,13 @@
         <v>포킹(four king)</v>
       </c>
       <c r="C70" t="str">
-        <v>B</v>
+        <v>팀원2</v>
       </c>
       <c r="D70" t="str">
-        <v>팀원2</v>
+        <v>claire.yz</v>
       </c>
       <c r="E70" t="str">
-        <v>claire.yz</v>
-      </c>
-      <c r="F70" t="str">
-        <v>593024</v>
+        <v/>
       </c>
     </row>
     <row r="71">
@@ -1818,16 +1607,13 @@
         <v>포킹(four king)</v>
       </c>
       <c r="C71" t="str">
-        <v>B</v>
+        <v>팀원3</v>
       </c>
       <c r="D71" t="str">
-        <v>팀원3</v>
+        <v>joy.ur</v>
       </c>
       <c r="E71" t="str">
-        <v>joy.ur</v>
-      </c>
-      <c r="F71" t="str">
-        <v>375693</v>
+        <v/>
       </c>
     </row>
     <row r="72">
@@ -1838,16 +1624,13 @@
         <v>포킹(four king)</v>
       </c>
       <c r="C72" t="str">
-        <v>B</v>
+        <v>팀원4</v>
       </c>
       <c r="D72" t="str">
-        <v>팀원4</v>
+        <v>hayden.cloud</v>
       </c>
       <c r="E72" t="str">
-        <v>hayden.cloud</v>
-      </c>
-      <c r="F72" t="str">
-        <v>849448</v>
+        <v/>
       </c>
     </row>
     <row r="73">
@@ -1858,16 +1641,13 @@
         <v>리밸런싱</v>
       </c>
       <c r="C73" t="str">
-        <v>C</v>
+        <v>팀장</v>
       </c>
       <c r="D73" t="str">
-        <v>팀장</v>
+        <v>todd.rsp</v>
       </c>
       <c r="E73" t="str">
-        <v>todd.rsp</v>
-      </c>
-      <c r="F73" t="str">
-        <v>304613</v>
+        <v/>
       </c>
     </row>
     <row r="74">
@@ -1878,16 +1658,13 @@
         <v>리밸런싱</v>
       </c>
       <c r="C74" t="str">
-        <v>C</v>
+        <v>팀원2</v>
       </c>
       <c r="D74" t="str">
-        <v>팀원2</v>
+        <v>harry.ellaton</v>
       </c>
       <c r="E74" t="str">
-        <v>harry.ellaton</v>
-      </c>
-      <c r="F74" t="str">
-        <v>804247</v>
+        <v/>
       </c>
     </row>
     <row r="75">
@@ -1898,16 +1675,13 @@
         <v>리밸런싱</v>
       </c>
       <c r="C75" t="str">
-        <v>C</v>
+        <v>팀원3</v>
       </c>
       <c r="D75" t="str">
-        <v>팀원3</v>
+        <v>light.y</v>
       </c>
       <c r="E75" t="str">
-        <v>light.y</v>
-      </c>
-      <c r="F75" t="str">
-        <v>472843</v>
+        <v/>
       </c>
     </row>
     <row r="76">
@@ -1918,16 +1692,13 @@
         <v>리밸런싱</v>
       </c>
       <c r="C76" t="str">
-        <v>C</v>
+        <v>팀원4</v>
       </c>
       <c r="D76" t="str">
-        <v>팀원4</v>
+        <v>silva.nus</v>
       </c>
       <c r="E76" t="str">
-        <v>silva.nus</v>
-      </c>
-      <c r="F76" t="str">
-        <v>668055</v>
+        <v/>
       </c>
     </row>
     <row r="77">
@@ -1938,16 +1709,13 @@
         <v>세2디</v>
       </c>
       <c r="C77" t="str">
-        <v>C</v>
+        <v>팀장</v>
       </c>
       <c r="D77" t="str">
-        <v>팀장</v>
+        <v>judy.hey</v>
       </c>
       <c r="E77" t="str">
-        <v>judy.hey</v>
-      </c>
-      <c r="F77" t="str">
-        <v>585862</v>
+        <v/>
       </c>
     </row>
     <row r="78">
@@ -1958,16 +1726,13 @@
         <v>세2디</v>
       </c>
       <c r="C78" t="str">
-        <v>C</v>
+        <v>팀원2</v>
       </c>
       <c r="D78" t="str">
-        <v>팀원2</v>
+        <v>sage.green</v>
       </c>
       <c r="E78" t="str">
-        <v>sage.green</v>
-      </c>
-      <c r="F78" t="str">
-        <v>438504</v>
+        <v/>
       </c>
     </row>
     <row r="79">
@@ -1978,16 +1743,13 @@
         <v>세2디</v>
       </c>
       <c r="C79" t="str">
-        <v>C</v>
+        <v>팀원3</v>
       </c>
       <c r="D79" t="str">
-        <v>팀원3</v>
+        <v>wendy.house</v>
       </c>
       <c r="E79" t="str">
-        <v>wendy.house</v>
-      </c>
-      <c r="F79" t="str">
-        <v>494106</v>
+        <v/>
       </c>
     </row>
     <row r="80">
@@ -1998,16 +1760,13 @@
         <v>백현동532</v>
       </c>
       <c r="C80" t="str">
-        <v>C</v>
+        <v>팀장</v>
       </c>
       <c r="D80" t="str">
-        <v>팀장</v>
+        <v>coca.cola</v>
       </c>
       <c r="E80" t="str">
-        <v>coca.cola</v>
-      </c>
-      <c r="F80" t="str">
-        <v>629134</v>
+        <v/>
       </c>
     </row>
     <row r="81">
@@ -2018,16 +1777,13 @@
         <v>백현동532</v>
       </c>
       <c r="C81" t="str">
-        <v>C</v>
+        <v>팀원2</v>
       </c>
       <c r="D81" t="str">
-        <v>팀원2</v>
+        <v>mark.sehun</v>
       </c>
       <c r="E81" t="str">
-        <v>mark.sehun</v>
-      </c>
-      <c r="F81" t="str">
-        <v>180980</v>
+        <v/>
       </c>
     </row>
     <row r="82">
@@ -2038,16 +1794,13 @@
         <v>백현동532</v>
       </c>
       <c r="C82" t="str">
-        <v>C</v>
+        <v>팀원3</v>
       </c>
       <c r="D82" t="str">
-        <v>팀원3</v>
+        <v>stak.bucks</v>
       </c>
       <c r="E82" t="str">
-        <v>stak.bucks</v>
-      </c>
-      <c r="F82" t="str">
-        <v>309658</v>
+        <v/>
       </c>
     </row>
     <row r="83">
@@ -2058,16 +1811,13 @@
         <v>백현동532</v>
       </c>
       <c r="C83" t="str">
-        <v>C</v>
+        <v>팀원4</v>
       </c>
       <c r="D83" t="str">
-        <v>팀원4</v>
+        <v>martin.sw</v>
       </c>
       <c r="E83" t="str">
-        <v>martin.sw</v>
-      </c>
-      <c r="F83" t="str">
-        <v>420432</v>
+        <v/>
       </c>
     </row>
     <row r="84">
@@ -2078,16 +1828,13 @@
         <v>AI야 우리 팀명 정해조</v>
       </c>
       <c r="C84" t="str">
-        <v>C</v>
+        <v>팀장</v>
       </c>
       <c r="D84" t="str">
-        <v>팀장</v>
+        <v>kay.one</v>
       </c>
       <c r="E84" t="str">
-        <v>kay.one</v>
-      </c>
-      <c r="F84" t="str">
-        <v>190592</v>
+        <v/>
       </c>
     </row>
     <row r="85">
@@ -2098,16 +1845,13 @@
         <v>AI야 우리 팀명 정해조</v>
       </c>
       <c r="C85" t="str">
-        <v>C</v>
+        <v>팀원2</v>
       </c>
       <c r="D85" t="str">
-        <v>팀원2</v>
+        <v>parker.s</v>
       </c>
       <c r="E85" t="str">
-        <v>parker.s</v>
-      </c>
-      <c r="F85" t="str">
-        <v>403734</v>
+        <v/>
       </c>
     </row>
     <row r="86">
@@ -2118,16 +1862,13 @@
         <v>AI야 우리 팀명 정해조</v>
       </c>
       <c r="C86" t="str">
-        <v>C</v>
+        <v>팀원3</v>
       </c>
       <c r="D86" t="str">
-        <v>팀원3</v>
+        <v>captain.kr</v>
       </c>
       <c r="E86" t="str">
-        <v>captain.kr</v>
-      </c>
-      <c r="F86" t="str">
-        <v>894902</v>
+        <v/>
       </c>
     </row>
     <row r="87">
@@ -2138,16 +1879,13 @@
         <v>AI야 우리 팀명 정해조</v>
       </c>
       <c r="C87" t="str">
-        <v>C</v>
+        <v>팀원4</v>
       </c>
       <c r="D87" t="str">
-        <v>팀원4</v>
+        <v>rhys.kim</v>
       </c>
       <c r="E87" t="str">
-        <v>rhys.kim</v>
-      </c>
-      <c r="F87" t="str">
-        <v>442944</v>
+        <v/>
       </c>
     </row>
     <row r="88">
@@ -2158,16 +1896,13 @@
         <v>제페토</v>
       </c>
       <c r="C88" t="str">
-        <v>C</v>
+        <v>팀장</v>
       </c>
       <c r="D88" t="str">
-        <v>팀장</v>
+        <v>tora.kim</v>
       </c>
       <c r="E88" t="str">
-        <v>tora.kim</v>
-      </c>
-      <c r="F88" t="str">
-        <v>129652</v>
+        <v/>
       </c>
     </row>
     <row r="89">
@@ -2178,16 +1913,13 @@
         <v>제페토</v>
       </c>
       <c r="C89" t="str">
-        <v>C</v>
+        <v>팀원2</v>
       </c>
       <c r="D89" t="str">
-        <v>팀원2</v>
+        <v>jake.ui</v>
       </c>
       <c r="E89" t="str">
-        <v>jake.ui</v>
-      </c>
-      <c r="F89" t="str">
-        <v>536453</v>
+        <v/>
       </c>
     </row>
     <row r="90">
@@ -2198,16 +1930,13 @@
         <v>제페토</v>
       </c>
       <c r="C90" t="str">
-        <v>C</v>
+        <v>팀원3</v>
       </c>
       <c r="D90" t="str">
-        <v>팀원3</v>
+        <v>jerry.dy</v>
       </c>
       <c r="E90" t="str">
-        <v>jerry.dy</v>
-      </c>
-      <c r="F90" t="str">
-        <v>418081</v>
+        <v/>
       </c>
     </row>
     <row r="91">
@@ -2218,16 +1947,13 @@
         <v>헬로카봇</v>
       </c>
       <c r="C91" t="str">
-        <v>C</v>
+        <v>팀장</v>
       </c>
       <c r="D91" t="str">
-        <v>팀장</v>
+        <v>ella.7</v>
       </c>
       <c r="E91" t="str">
-        <v>ella.7</v>
-      </c>
-      <c r="F91" t="str">
-        <v>936436</v>
+        <v/>
       </c>
     </row>
     <row r="92">
@@ -2238,16 +1964,13 @@
         <v>헬로카봇</v>
       </c>
       <c r="C92" t="str">
-        <v>C</v>
+        <v>팀원2</v>
       </c>
       <c r="D92" t="str">
-        <v>팀원2</v>
+        <v>benny.1013</v>
       </c>
       <c r="E92" t="str">
-        <v>benny.1013</v>
-      </c>
-      <c r="F92" t="str">
-        <v>937043</v>
+        <v/>
       </c>
     </row>
     <row r="93">
@@ -2258,16 +1981,13 @@
         <v>헬로카봇</v>
       </c>
       <c r="C93" t="str">
-        <v>C</v>
+        <v>팀원3</v>
       </c>
       <c r="D93" t="str">
-        <v>팀원3</v>
+        <v>dwayne.jung</v>
       </c>
       <c r="E93" t="str">
-        <v>dwayne.jung</v>
-      </c>
-      <c r="F93" t="str">
-        <v>891866</v>
+        <v/>
       </c>
     </row>
     <row r="94">
@@ -2278,16 +1998,13 @@
         <v>OMMA(Oracle/MySQL/MongoDB/Altibase)</v>
       </c>
       <c r="C94" t="str">
-        <v>C</v>
+        <v>팀장</v>
       </c>
       <c r="D94" t="str">
-        <v>팀장</v>
+        <v>frang.sua</v>
       </c>
       <c r="E94" t="str">
-        <v>frang.sua</v>
-      </c>
-      <c r="F94" t="str">
-        <v>395751</v>
+        <v/>
       </c>
     </row>
     <row r="95">
@@ -2298,16 +2015,13 @@
         <v>OMMA(Oracle/MySQL/MongoDB/Altibase)</v>
       </c>
       <c r="C95" t="str">
-        <v>C</v>
+        <v>팀원2</v>
       </c>
       <c r="D95" t="str">
-        <v>팀원2</v>
+        <v>david.25</v>
       </c>
       <c r="E95" t="str">
-        <v>david.25</v>
-      </c>
-      <c r="F95" t="str">
-        <v>142525</v>
+        <v/>
       </c>
     </row>
     <row r="96">
@@ -2318,16 +2032,13 @@
         <v>WT</v>
       </c>
       <c r="C96" t="str">
-        <v>C</v>
+        <v>팀장</v>
       </c>
       <c r="D96" t="str">
-        <v>팀장</v>
+        <v>matthew.home</v>
       </c>
       <c r="E96" t="str">
-        <v>matthew.home</v>
-      </c>
-      <c r="F96" t="str">
-        <v>269939</v>
+        <v/>
       </c>
     </row>
     <row r="97">
@@ -2338,16 +2049,13 @@
         <v>WT</v>
       </c>
       <c r="C97" t="str">
-        <v>C</v>
+        <v>팀원2</v>
       </c>
       <c r="D97" t="str">
-        <v>팀원2</v>
+        <v>tony.arc</v>
       </c>
       <c r="E97" t="str">
-        <v>tony.arc</v>
-      </c>
-      <c r="F97" t="str">
-        <v>413613</v>
+        <v/>
       </c>
     </row>
     <row r="98">
@@ -2358,16 +2066,13 @@
         <v>HackRush</v>
       </c>
       <c r="C98" t="str">
-        <v>C</v>
+        <v>팀장</v>
       </c>
       <c r="D98" t="str">
-        <v>팀장</v>
+        <v>joshua.yoon</v>
       </c>
       <c r="E98" t="str">
-        <v>joshua.yoon</v>
-      </c>
-      <c r="F98" t="str">
-        <v>171015</v>
+        <v/>
       </c>
     </row>
     <row r="99">
@@ -2378,16 +2083,13 @@
         <v>HackRush</v>
       </c>
       <c r="C99" t="str">
-        <v>C</v>
+        <v>팀원2</v>
       </c>
       <c r="D99" t="str">
-        <v>팀원2</v>
+        <v>kaia.toast</v>
       </c>
       <c r="E99" t="str">
-        <v>kaia.toast</v>
-      </c>
-      <c r="F99" t="str">
-        <v>855108</v>
+        <v/>
       </c>
     </row>
     <row r="100">
@@ -2398,16 +2100,13 @@
         <v>HackRush</v>
       </c>
       <c r="C100" t="str">
-        <v>C</v>
+        <v>팀원3</v>
       </c>
       <c r="D100" t="str">
-        <v>팀원3</v>
+        <v>juno.choi</v>
       </c>
       <c r="E100" t="str">
-        <v>juno.choi</v>
-      </c>
-      <c r="F100" t="str">
-        <v>438922</v>
+        <v/>
       </c>
     </row>
     <row r="101">
@@ -2418,16 +2117,13 @@
         <v>HackRush</v>
       </c>
       <c r="C101" t="str">
-        <v>C</v>
+        <v>팀원4</v>
       </c>
       <c r="D101" t="str">
-        <v>팀원4</v>
+        <v>kai.09</v>
       </c>
       <c r="E101" t="str">
-        <v>kai.09</v>
-      </c>
-      <c r="F101" t="str">
-        <v>898533</v>
+        <v/>
       </c>
     </row>
     <row r="102">
@@ -2438,16 +2134,13 @@
         <v>s팀과제리2</v>
       </c>
       <c r="C102" t="str">
-        <v>C</v>
+        <v>팀장</v>
       </c>
       <c r="D102" t="str">
-        <v>팀장</v>
+        <v>steam.na</v>
       </c>
       <c r="E102" t="str">
-        <v>steam.na</v>
-      </c>
-      <c r="F102" t="str">
-        <v>155435</v>
+        <v/>
       </c>
     </row>
     <row r="103">
@@ -2458,21 +2151,18 @@
         <v>s팀과제리2</v>
       </c>
       <c r="C103" t="str">
-        <v>C</v>
+        <v>팀원2</v>
       </c>
       <c r="D103" t="str">
-        <v>팀원2</v>
+        <v>jarry.han</v>
       </c>
       <c r="E103" t="str">
-        <v>jarry.han</v>
-      </c>
-      <c r="F103" t="str">
-        <v>571979</v>
+        <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F103"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E103"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Add password authentication for admin and results pages
- Add password protection (hack2025) for /admin and /results pages
- Enhance security by preventing unauthorized access via URL patterns
- Remove '홈으로 돌아가기' buttons from participant voting pages
- Fix authentication code validation and error messages
- Update team data with authentication codes
- Improve admin dashboard voter management display
</commit_message>
<xml_diff>
--- a/auth-codes.xlsx
+++ b/auth-codes.xlsx
@@ -440,7 +440,7 @@
         <v>logan.g</v>
       </c>
       <c r="E2" t="str">
-        <v/>
+        <v>980380</v>
       </c>
     </row>
     <row r="3">
@@ -457,7 +457,7 @@
         <v>oregon.a</v>
       </c>
       <c r="E3" t="str">
-        <v/>
+        <v>869215</v>
       </c>
     </row>
     <row r="4">
@@ -474,7 +474,7 @@
         <v>alicia.a</v>
       </c>
       <c r="E4" t="str">
-        <v/>
+        <v>962236</v>
       </c>
     </row>
     <row r="5">
@@ -491,7 +491,7 @@
         <v>sean.baek</v>
       </c>
       <c r="E5" t="str">
-        <v/>
+        <v>464023</v>
       </c>
     </row>
     <row r="6">
@@ -508,7 +508,7 @@
         <v>leo.bing</v>
       </c>
       <c r="E6" t="str">
-        <v/>
+        <v>936997</v>
       </c>
     </row>
     <row r="7">
@@ -525,7 +525,7 @@
         <v>ryder.wind</v>
       </c>
       <c r="E7" t="str">
-        <v/>
+        <v>787965</v>
       </c>
     </row>
     <row r="8">
@@ -542,7 +542,7 @@
         <v>tak.haru</v>
       </c>
       <c r="E8" t="str">
-        <v/>
+        <v>994515</v>
       </c>
     </row>
     <row r="9">
@@ -559,7 +559,7 @@
         <v>lou.j</v>
       </c>
       <c r="E9" t="str">
-        <v/>
+        <v>346857</v>
       </c>
     </row>
     <row r="10">
@@ -576,7 +576,7 @@
         <v>james.yu</v>
       </c>
       <c r="E10" t="str">
-        <v/>
+        <v>730438</v>
       </c>
     </row>
     <row r="11">
@@ -593,7 +593,7 @@
         <v>miles.stone</v>
       </c>
       <c r="E11" t="str">
-        <v/>
+        <v>389118</v>
       </c>
     </row>
     <row r="12">
@@ -610,7 +610,7 @@
         <v>ogong.cloud</v>
       </c>
       <c r="E12" t="str">
-        <v/>
+        <v>729012</v>
       </c>
     </row>
     <row r="13">
@@ -627,7 +627,7 @@
         <v>eli.94</v>
       </c>
       <c r="E13" t="str">
-        <v/>
+        <v>519737</v>
       </c>
     </row>
     <row r="14">
@@ -644,7 +644,7 @@
         <v>ud.zip</v>
       </c>
       <c r="E14" t="str">
-        <v/>
+        <v>385432</v>
       </c>
     </row>
     <row r="15">
@@ -661,7 +661,7 @@
         <v>lucas.nova</v>
       </c>
       <c r="E15" t="str">
-        <v/>
+        <v>953153</v>
       </c>
     </row>
     <row r="16">
@@ -678,7 +678,7 @@
         <v>joy.wooyakko</v>
       </c>
       <c r="E16" t="str">
-        <v/>
+        <v>628249</v>
       </c>
     </row>
     <row r="17">
@@ -695,7 +695,7 @@
         <v>jackson.yoon</v>
       </c>
       <c r="E17" t="str">
-        <v/>
+        <v>444923</v>
       </c>
     </row>
     <row r="18">
@@ -712,7 +712,7 @@
         <v>evin.yj</v>
       </c>
       <c r="E18" t="str">
-        <v/>
+        <v>176475</v>
       </c>
     </row>
     <row r="19">
@@ -729,7 +729,7 @@
         <v>vito.kim</v>
       </c>
       <c r="E19" t="str">
-        <v/>
+        <v>139507</v>
       </c>
     </row>
     <row r="20">
@@ -746,7 +746,7 @@
         <v>nyx.domi</v>
       </c>
       <c r="E20" t="str">
-        <v/>
+        <v>738484</v>
       </c>
     </row>
     <row r="21">
@@ -763,7 +763,7 @@
         <v>ian.hyuek</v>
       </c>
       <c r="E21" t="str">
-        <v/>
+        <v>834355</v>
       </c>
     </row>
     <row r="22">
@@ -780,7 +780,7 @@
         <v>gide.yso</v>
       </c>
       <c r="E22" t="str">
-        <v/>
+        <v>864841</v>
       </c>
     </row>
     <row r="23">
@@ -797,7 +797,7 @@
         <v>rian.bow</v>
       </c>
       <c r="E23" t="str">
-        <v/>
+        <v>171803</v>
       </c>
     </row>
     <row r="24">
@@ -814,7 +814,7 @@
         <v>bacchus.f</v>
       </c>
       <c r="E24" t="str">
-        <v/>
+        <v>181586</v>
       </c>
     </row>
     <row r="25">
@@ -831,7 +831,7 @@
         <v>derek.young</v>
       </c>
       <c r="E25" t="str">
-        <v/>
+        <v>155354</v>
       </c>
     </row>
     <row r="26">
@@ -848,7 +848,7 @@
         <v>steve.play</v>
       </c>
       <c r="E26" t="str">
-        <v/>
+        <v>213473</v>
       </c>
     </row>
     <row r="27">
@@ -865,7 +865,7 @@
         <v>terra.bite</v>
       </c>
       <c r="E27" t="str">
-        <v/>
+        <v>546779</v>
       </c>
     </row>
     <row r="28">
@@ -882,7 +882,7 @@
         <v>khloe.wynn</v>
       </c>
       <c r="E28" t="str">
-        <v/>
+        <v>768395</v>
       </c>
     </row>
     <row r="29">
@@ -899,7 +899,7 @@
         <v>hugh.1123</v>
       </c>
       <c r="E29" t="str">
-        <v/>
+        <v>485369</v>
       </c>
     </row>
     <row r="30">
@@ -916,7 +916,7 @@
         <v>lina.a</v>
       </c>
       <c r="E30" t="str">
-        <v/>
+        <v>585172</v>
       </c>
     </row>
     <row r="31">
@@ -933,7 +933,7 @@
         <v>bell.na</v>
       </c>
       <c r="E31" t="str">
-        <v/>
+        <v>903143</v>
       </c>
     </row>
     <row r="32">
@@ -950,7 +950,7 @@
         <v>woody.n</v>
       </c>
       <c r="E32" t="str">
-        <v/>
+        <v>173650</v>
       </c>
     </row>
     <row r="33">
@@ -967,7 +967,7 @@
         <v>rick.9</v>
       </c>
       <c r="E33" t="str">
-        <v/>
+        <v>208394</v>
       </c>
     </row>
     <row r="34">
@@ -984,7 +984,7 @@
         <v>peter.hoon</v>
       </c>
       <c r="E34" t="str">
-        <v/>
+        <v>768612</v>
       </c>
     </row>
     <row r="35">
@@ -1001,7 +1001,7 @@
         <v>adam.min</v>
       </c>
       <c r="E35" t="str">
-        <v/>
+        <v>907900</v>
       </c>
     </row>
     <row r="36">
@@ -1018,7 +1018,7 @@
         <v>maison.sun</v>
       </c>
       <c r="E36" t="str">
-        <v/>
+        <v>704897</v>
       </c>
     </row>
     <row r="37">
@@ -1035,7 +1035,7 @@
         <v>aaron.bless</v>
       </c>
       <c r="E37" t="str">
-        <v/>
+        <v>597581</v>
       </c>
     </row>
     <row r="38">
@@ -1052,7 +1052,7 @@
         <v>andrew.j88</v>
       </c>
       <c r="E38" t="str">
-        <v/>
+        <v>854670</v>
       </c>
     </row>
     <row r="39">
@@ -1069,7 +1069,7 @@
         <v>harry.2024</v>
       </c>
       <c r="E39" t="str">
-        <v/>
+        <v>745577</v>
       </c>
     </row>
     <row r="40">
@@ -1086,7 +1086,7 @@
         <v>john.al</v>
       </c>
       <c r="E40" t="str">
-        <v/>
+        <v>612452</v>
       </c>
     </row>
     <row r="41">
@@ -1103,7 +1103,7 @@
         <v>bella.nam</v>
       </c>
       <c r="E41" t="str">
-        <v/>
+        <v>898091</v>
       </c>
     </row>
     <row r="42">
@@ -1120,7 +1120,7 @@
         <v>ico.dev</v>
       </c>
       <c r="E42" t="str">
-        <v/>
+        <v>126394</v>
       </c>
     </row>
     <row r="43">
@@ -1137,7 +1137,7 @@
         <v>danny.l</v>
       </c>
       <c r="E43" t="str">
-        <v/>
+        <v>418642</v>
       </c>
     </row>
     <row r="44">
@@ -1154,7 +1154,7 @@
         <v>jaclyn.n</v>
       </c>
       <c r="E44" t="str">
-        <v/>
+        <v>541281</v>
       </c>
     </row>
     <row r="45">
@@ -1171,7 +1171,7 @@
         <v>lucas.link</v>
       </c>
       <c r="E45" t="str">
-        <v/>
+        <v>712603</v>
       </c>
     </row>
     <row r="46">
@@ -1188,7 +1188,7 @@
         <v>cyan.jade</v>
       </c>
       <c r="E46" t="str">
-        <v/>
+        <v>910607</v>
       </c>
     </row>
     <row r="47">
@@ -1205,7 +1205,7 @@
         <v>theo.jo</v>
       </c>
       <c r="E47" t="str">
-        <v/>
+        <v>455458</v>
       </c>
     </row>
     <row r="48">
@@ -1222,7 +1222,7 @@
         <v>jor.dy</v>
       </c>
       <c r="E48" t="str">
-        <v/>
+        <v>253530</v>
       </c>
     </row>
     <row r="49">
@@ -1239,7 +1239,7 @@
         <v>walker.kind</v>
       </c>
       <c r="E49" t="str">
-        <v/>
+        <v>839338</v>
       </c>
     </row>
     <row r="50">
@@ -1256,7 +1256,7 @@
         <v>orsay.art</v>
       </c>
       <c r="E50" t="str">
-        <v/>
+        <v>109671</v>
       </c>
     </row>
     <row r="51">
@@ -1273,7 +1273,7 @@
         <v>john.athan</v>
       </c>
       <c r="E51" t="str">
-        <v/>
+        <v>304480</v>
       </c>
     </row>
     <row r="52">
@@ -1290,7 +1290,7 @@
         <v>erin.u</v>
       </c>
       <c r="E52" t="str">
-        <v/>
+        <v>222609</v>
       </c>
     </row>
     <row r="53">
@@ -1307,7 +1307,7 @@
         <v>sean.cm</v>
       </c>
       <c r="E53" t="str">
-        <v/>
+        <v>349320</v>
       </c>
     </row>
     <row r="54">
@@ -1324,7 +1324,7 @@
         <v>zero.a</v>
       </c>
       <c r="E54" t="str">
-        <v/>
+        <v>538007</v>
       </c>
     </row>
     <row r="55">
@@ -1341,7 +1341,7 @@
         <v>barack.abama</v>
       </c>
       <c r="E55" t="str">
-        <v/>
+        <v>266802</v>
       </c>
     </row>
     <row r="56">
@@ -1358,7 +1358,7 @@
         <v>heidi.0929</v>
       </c>
       <c r="E56" t="str">
-        <v/>
+        <v>889105</v>
       </c>
     </row>
     <row r="57">
@@ -1375,7 +1375,7 @@
         <v>marc.shin</v>
       </c>
       <c r="E57" t="str">
-        <v/>
+        <v>370184</v>
       </c>
     </row>
     <row r="58">
@@ -1392,7 +1392,7 @@
         <v>brett.bang</v>
       </c>
       <c r="E58" t="str">
-        <v/>
+        <v>358021</v>
       </c>
     </row>
     <row r="59">
@@ -1409,7 +1409,7 @@
         <v>anna.iam</v>
       </c>
       <c r="E59" t="str">
-        <v/>
+        <v>507495</v>
       </c>
     </row>
     <row r="60">
@@ -1426,7 +1426,7 @@
         <v>kaya.daystar</v>
       </c>
       <c r="E60" t="str">
-        <v/>
+        <v>396873</v>
       </c>
     </row>
     <row r="61">
@@ -1443,7 +1443,7 @@
         <v>rose.viva</v>
       </c>
       <c r="E61" t="str">
-        <v/>
+        <v>678386</v>
       </c>
     </row>
     <row r="62">
@@ -1460,7 +1460,7 @@
         <v>millie.y</v>
       </c>
       <c r="E62" t="str">
-        <v/>
+        <v>604968</v>
       </c>
     </row>
     <row r="63">
@@ -1477,7 +1477,7 @@
         <v>halang.g</v>
       </c>
       <c r="E63" t="str">
-        <v/>
+        <v>231300</v>
       </c>
     </row>
     <row r="64">
@@ -1494,7 +1494,7 @@
         <v>thru.shine</v>
       </c>
       <c r="E64" t="str">
-        <v/>
+        <v>375395</v>
       </c>
     </row>
     <row r="65">
@@ -1511,7 +1511,7 @@
         <v>ellen.aries</v>
       </c>
       <c r="E65" t="str">
-        <v/>
+        <v>312840</v>
       </c>
     </row>
     <row r="66">
@@ -1528,7 +1528,7 @@
         <v>jerome.u</v>
       </c>
       <c r="E66" t="str">
-        <v/>
+        <v>149778</v>
       </c>
     </row>
     <row r="67">
@@ -1545,7 +1545,7 @@
         <v>leo.v</v>
       </c>
       <c r="E67" t="str">
-        <v/>
+        <v>675561</v>
       </c>
     </row>
     <row r="68">
@@ -1562,7 +1562,7 @@
         <v>jayden.hue</v>
       </c>
       <c r="E68" t="str">
-        <v/>
+        <v>985239</v>
       </c>
     </row>
     <row r="69">
@@ -1579,7 +1579,7 @@
         <v>sienna.on</v>
       </c>
       <c r="E69" t="str">
-        <v/>
+        <v>305000</v>
       </c>
     </row>
     <row r="70">
@@ -1596,7 +1596,7 @@
         <v>claire.yz</v>
       </c>
       <c r="E70" t="str">
-        <v/>
+        <v>491445</v>
       </c>
     </row>
     <row r="71">
@@ -1613,7 +1613,7 @@
         <v>joy.ur</v>
       </c>
       <c r="E71" t="str">
-        <v/>
+        <v>217039</v>
       </c>
     </row>
     <row r="72">
@@ -1630,7 +1630,7 @@
         <v>hayden.cloud</v>
       </c>
       <c r="E72" t="str">
-        <v/>
+        <v>962823</v>
       </c>
     </row>
     <row r="73">
@@ -1647,7 +1647,7 @@
         <v>todd.rsp</v>
       </c>
       <c r="E73" t="str">
-        <v/>
+        <v>814247</v>
       </c>
     </row>
     <row r="74">
@@ -1664,7 +1664,7 @@
         <v>harry.ellaton</v>
       </c>
       <c r="E74" t="str">
-        <v/>
+        <v>662672</v>
       </c>
     </row>
     <row r="75">
@@ -1681,7 +1681,7 @@
         <v>light.y</v>
       </c>
       <c r="E75" t="str">
-        <v/>
+        <v>737056</v>
       </c>
     </row>
     <row r="76">
@@ -1698,7 +1698,7 @@
         <v>silva.nus</v>
       </c>
       <c r="E76" t="str">
-        <v/>
+        <v>106699</v>
       </c>
     </row>
     <row r="77">
@@ -1715,7 +1715,7 @@
         <v>judy.hey</v>
       </c>
       <c r="E77" t="str">
-        <v/>
+        <v>728342</v>
       </c>
     </row>
     <row r="78">
@@ -1732,7 +1732,7 @@
         <v>sage.green</v>
       </c>
       <c r="E78" t="str">
-        <v/>
+        <v>989269</v>
       </c>
     </row>
     <row r="79">
@@ -1749,7 +1749,7 @@
         <v>wendy.house</v>
       </c>
       <c r="E79" t="str">
-        <v/>
+        <v>948420</v>
       </c>
     </row>
     <row r="80">
@@ -1766,7 +1766,7 @@
         <v>coca.cola</v>
       </c>
       <c r="E80" t="str">
-        <v/>
+        <v>183149</v>
       </c>
     </row>
     <row r="81">
@@ -1783,7 +1783,7 @@
         <v>mark.sehun</v>
       </c>
       <c r="E81" t="str">
-        <v/>
+        <v>691711</v>
       </c>
     </row>
     <row r="82">
@@ -1800,7 +1800,7 @@
         <v>stak.bucks</v>
       </c>
       <c r="E82" t="str">
-        <v/>
+        <v>497244</v>
       </c>
     </row>
     <row r="83">
@@ -1817,7 +1817,7 @@
         <v>martin.sw</v>
       </c>
       <c r="E83" t="str">
-        <v/>
+        <v>656516</v>
       </c>
     </row>
     <row r="84">
@@ -1834,7 +1834,7 @@
         <v>kay.one</v>
       </c>
       <c r="E84" t="str">
-        <v/>
+        <v>931834</v>
       </c>
     </row>
     <row r="85">
@@ -1851,7 +1851,7 @@
         <v>parker.s</v>
       </c>
       <c r="E85" t="str">
-        <v/>
+        <v>208546</v>
       </c>
     </row>
     <row r="86">
@@ -1868,7 +1868,7 @@
         <v>captain.kr</v>
       </c>
       <c r="E86" t="str">
-        <v/>
+        <v>803195</v>
       </c>
     </row>
     <row r="87">
@@ -1885,7 +1885,7 @@
         <v>rhys.kim</v>
       </c>
       <c r="E87" t="str">
-        <v/>
+        <v>136982</v>
       </c>
     </row>
     <row r="88">
@@ -1902,7 +1902,7 @@
         <v>tora.kim</v>
       </c>
       <c r="E88" t="str">
-        <v/>
+        <v>405446</v>
       </c>
     </row>
     <row r="89">
@@ -1919,7 +1919,7 @@
         <v>jake.ui</v>
       </c>
       <c r="E89" t="str">
-        <v/>
+        <v>132462</v>
       </c>
     </row>
     <row r="90">
@@ -1936,7 +1936,7 @@
         <v>jerry.dy</v>
       </c>
       <c r="E90" t="str">
-        <v/>
+        <v>411804</v>
       </c>
     </row>
     <row r="91">
@@ -1953,7 +1953,7 @@
         <v>ella.7</v>
       </c>
       <c r="E91" t="str">
-        <v/>
+        <v>367603</v>
       </c>
     </row>
     <row r="92">
@@ -1970,7 +1970,7 @@
         <v>benny.1013</v>
       </c>
       <c r="E92" t="str">
-        <v/>
+        <v>258910</v>
       </c>
     </row>
     <row r="93">
@@ -1987,7 +1987,7 @@
         <v>dwayne.jung</v>
       </c>
       <c r="E93" t="str">
-        <v/>
+        <v>997294</v>
       </c>
     </row>
     <row r="94">
@@ -2004,7 +2004,7 @@
         <v>frang.sua</v>
       </c>
       <c r="E94" t="str">
-        <v/>
+        <v>647916</v>
       </c>
     </row>
     <row r="95">
@@ -2021,7 +2021,7 @@
         <v>david.25</v>
       </c>
       <c r="E95" t="str">
-        <v/>
+        <v>363254</v>
       </c>
     </row>
     <row r="96">
@@ -2038,7 +2038,7 @@
         <v>matthew.home</v>
       </c>
       <c r="E96" t="str">
-        <v/>
+        <v>247307</v>
       </c>
     </row>
     <row r="97">
@@ -2055,7 +2055,7 @@
         <v>tony.arc</v>
       </c>
       <c r="E97" t="str">
-        <v/>
+        <v>941276</v>
       </c>
     </row>
     <row r="98">
@@ -2072,7 +2072,7 @@
         <v>joshua.yoon</v>
       </c>
       <c r="E98" t="str">
-        <v/>
+        <v>763535</v>
       </c>
     </row>
     <row r="99">
@@ -2089,7 +2089,7 @@
         <v>kaia.toast</v>
       </c>
       <c r="E99" t="str">
-        <v/>
+        <v>534988</v>
       </c>
     </row>
     <row r="100">
@@ -2106,7 +2106,7 @@
         <v>juno.choi</v>
       </c>
       <c r="E100" t="str">
-        <v/>
+        <v>785857</v>
       </c>
     </row>
     <row r="101">
@@ -2123,7 +2123,7 @@
         <v>kai.09</v>
       </c>
       <c r="E101" t="str">
-        <v/>
+        <v>459648</v>
       </c>
     </row>
     <row r="102">
@@ -2140,7 +2140,7 @@
         <v>steam.na</v>
       </c>
       <c r="E102" t="str">
-        <v/>
+        <v>695374</v>
       </c>
     </row>
     <row r="103">
@@ -2157,7 +2157,7 @@
         <v>jarry.han</v>
       </c>
       <c r="E103" t="str">
-        <v/>
+        <v>789268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>